<commit_message>
removed chars, work imgs, tiles, .wavs
</commit_message>
<xml_diff>
--- a/Dungeons of Gal'Darah.xlsx
+++ b/Dungeons of Gal'Darah.xlsx
@@ -1,38 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Andres\Developer\Dungeons of Gal'Darah (2.0)\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="18900" windowHeight="8190" tabRatio="616" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="18900" windowHeight="8190" tabRatio="616" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Items" sheetId="1" r:id="rId1"/>
-    <sheet name="Mob Sectors" sheetId="3" r:id="rId2"/>
-    <sheet name="Mob Sectors (2)" sheetId="7" r:id="rId3"/>
-    <sheet name="Lighting" sheetId="8" r:id="rId4"/>
-    <sheet name="Formula Test" sheetId="6" r:id="rId5"/>
+    <sheet name="Mob Sectors" sheetId="3" r:id="rId1"/>
+    <sheet name="Mob Sectors (2)" sheetId="7" r:id="rId2"/>
+    <sheet name="Lighting" sheetId="8" r:id="rId3"/>
+    <sheet name="Formula Test" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="40">
-  <si>
-    <t>Use</t>
-  </si>
-  <si>
-    <t>Iron Sword</t>
-  </si>
-  <si>
-    <t>Weapon</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
   <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>Health Potion</t>
   </si>
   <si>
     <t>First Test</t>
@@ -59,81 +51,6 @@
     <t>Column</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>NAME</t>
-  </si>
-  <si>
-    <t>STACKABLE</t>
-  </si>
-  <si>
-    <t>TYPE</t>
-  </si>
-  <si>
-    <t>EFFECT</t>
-  </si>
-  <si>
-    <t>SLOT</t>
-  </si>
-  <si>
-    <t>Variant</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>ITEMS</t>
-  </si>
-  <si>
-    <t>Equip</t>
-  </si>
-  <si>
-    <t>Heals for 50 HP.</t>
-  </si>
-  <si>
-    <t>Increases Att. By</t>
-  </si>
-  <si>
-    <t>Stone Sword</t>
-  </si>
-  <si>
-    <t>Gold Axe</t>
-  </si>
-  <si>
-    <t>Iron Axe</t>
-  </si>
-  <si>
-    <t>Stone Axe</t>
-  </si>
-  <si>
-    <t>Poison</t>
-  </si>
-  <si>
-    <t>Heals for 100 HP.</t>
-  </si>
-  <si>
-    <t>Heals for 200 HP.</t>
-  </si>
-  <si>
-    <t>Hurts for 20 HP.</t>
-  </si>
-  <si>
-    <t>Iron Plate</t>
-  </si>
-  <si>
-    <t>Iron Helm</t>
-  </si>
-  <si>
-    <t>Helmet</t>
-  </si>
-  <si>
-    <t>Chest</t>
-  </si>
-  <si>
     <t>Values</t>
   </si>
   <si>
@@ -143,8 +60,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,7 +78,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,14 +91,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="20">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -191,21 +102,6 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -458,16 +354,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -506,14 +405,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -523,28 +420,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -556,230 +441,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill>
@@ -852,27 +533,19 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A2:G13" totalsRowShown="0">
-  <autoFilter ref="A2:G13"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="ID"/>
-    <tableColumn id="2" name="NAME"/>
-    <tableColumn id="3" name="Variant"/>
-    <tableColumn id="4" name="STACKABLE"/>
-    <tableColumn id="5" name="TYPE"/>
-    <tableColumn id="6" name="EFFECT"/>
-    <tableColumn id="7" name="SLOT"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -914,7 +587,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -946,9 +619,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -980,6 +654,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1155,352 +830,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G16"/>
-  <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="D11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="19">
-        <v>10</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="19">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="19">
-        <v>11</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="19">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="F16" s="20"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="27" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.75" thickBot="1"/>
-    <row r="2" spans="1:27" ht="15.75" thickBot="1">
+    <row r="1" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -1568,9 +916,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B3" s="7">
         <v>9</v>
@@ -1661,9 +1009,9 @@
         <v>F</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="15.75" thickBot="1">
+    <row r="4" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B4" s="5">
         <v>5</v>
@@ -1754,7 +1102,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="15.75" thickBot="1">
+    <row r="5" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="4"/>
@@ -1843,12 +1191,12 @@
         <v>F</v>
       </c>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -1936,9 +1284,9 @@
         <v>F</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="15.75" thickBot="1">
+    <row r="7" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" s="7">
         <v>20</v>
@@ -2029,9 +1377,9 @@
         <v>F</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="15.75" thickBot="1">
+    <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8" s="5">
         <f>B7/10</f>
@@ -2123,7 +1471,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -2212,7 +1560,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2301,7 +1649,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2390,7 +1738,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="15.75" thickBot="1">
+    <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -2479,13 +1827,13 @@
         <v>F</v>
       </c>
     </row>
-    <row r="13" spans="1:27">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="B13" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
+      <c r="B13" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
       <c r="E13" s="1"/>
       <c r="G13" s="3">
         <v>11</v>
@@ -2571,7 +1919,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="14" spans="1:27">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1</v>
       </c>
@@ -2675,7 +2023,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>2</v>
       </c>
@@ -2779,7 +2127,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="16" spans="1:27">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>3</v>
       </c>
@@ -2883,7 +2231,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="15.75" thickBot="1">
+    <row r="17" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>4</v>
       </c>
@@ -2987,7 +2335,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="18" spans="1:27">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -3076,13 +2424,13 @@
         <v>F</v>
       </c>
     </row>
-    <row r="19" spans="1:27">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
+      <c r="B19" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
       <c r="E19" s="1"/>
       <c r="G19" s="3">
         <v>17</v>
@@ -3168,7 +2516,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="20" spans="1:27">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>1</v>
       </c>
@@ -3272,7 +2620,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="21" spans="1:27">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>2</v>
       </c>
@@ -3376,7 +2724,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="22" spans="1:27" ht="15.75" thickBot="1">
+    <row r="22" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>3</v>
       </c>
@@ -3480,7 +2828,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="23" spans="1:27">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>4</v>
       </c>
@@ -3507,18 +2855,18 @@
     <mergeCell ref="B19:D19"/>
   </mergeCells>
   <conditionalFormatting sqref="B14:E17 B20:E23">
-    <cfRule type="cellIs" dxfId="39" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"V"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:AA22">
-    <cfRule type="cellIs" dxfId="37" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"V"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3526,26 +2874,26 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="27" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.75" thickBot="1"/>
-    <row r="2" spans="1:27" ht="15.75" thickBot="1">
+    <row r="1" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -3613,9 +2961,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B3" s="7">
         <v>6</v>
@@ -3706,9 +3054,9 @@
         <v>F</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="15.75" thickBot="1">
+    <row r="4" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B4" s="5">
         <v>6</v>
@@ -3799,7 +3147,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="15.75" thickBot="1">
+    <row r="5" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="4"/>
@@ -3888,12 +3236,12 @@
         <v>F</v>
       </c>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -3981,9 +3329,9 @@
         <v>F</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="15.75" thickBot="1">
+    <row r="7" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" s="7">
         <v>20</v>
@@ -4013,70 +3361,70 @@
         <f t="shared" si="0"/>
         <v>F</v>
       </c>
-      <c r="M7" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>F</v>
-      </c>
-      <c r="N7" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>F</v>
-      </c>
-      <c r="O7" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>F</v>
-      </c>
-      <c r="P7" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>F</v>
-      </c>
-      <c r="Q7" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>F</v>
-      </c>
-      <c r="R7" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>F</v>
-      </c>
-      <c r="S7" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>F</v>
-      </c>
-      <c r="T7" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>F</v>
-      </c>
-      <c r="U7" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>F</v>
-      </c>
-      <c r="V7" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>F</v>
-      </c>
-      <c r="W7" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>F</v>
-      </c>
-      <c r="X7" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>F</v>
-      </c>
-      <c r="Y7" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>F</v>
-      </c>
-      <c r="Z7" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>F</v>
-      </c>
-      <c r="AA7" s="23" t="str">
+      <c r="M7" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>F</v>
+      </c>
+      <c r="N7" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>F</v>
+      </c>
+      <c r="O7" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>F</v>
+      </c>
+      <c r="P7" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>F</v>
+      </c>
+      <c r="Q7" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>F</v>
+      </c>
+      <c r="R7" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+      <c r="S7" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+      <c r="T7" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+      <c r="U7" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+      <c r="V7" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+      <c r="W7" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+      <c r="X7" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+      <c r="Y7" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+      <c r="Z7" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+      <c r="AA7" s="21" t="str">
         <f t="shared" si="1"/>
         <v>F</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="15.75" thickBot="1">
+    <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8" s="5">
         <f>B7/10</f>
@@ -4103,7 +3451,7 @@
         <f t="shared" si="0"/>
         <v>F</v>
       </c>
-      <c r="L8" s="21" t="str">
+      <c r="L8" s="19" t="str">
         <f t="shared" si="0"/>
         <v>F</v>
       </c>
@@ -4168,7 +3516,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -4192,7 +3540,7 @@
         <f t="shared" si="0"/>
         <v>F</v>
       </c>
-      <c r="L9" s="21" t="str">
+      <c r="L9" s="19" t="str">
         <f t="shared" si="0"/>
         <v>F</v>
       </c>
@@ -4257,7 +3605,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -4281,7 +3629,7 @@
         <f t="shared" si="0"/>
         <v>F</v>
       </c>
-      <c r="L10" s="21" t="str">
+      <c r="L10" s="19" t="str">
         <f t="shared" si="0"/>
         <v>F</v>
       </c>
@@ -4346,7 +3694,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -4370,7 +3718,7 @@
         <f t="shared" si="0"/>
         <v>F</v>
       </c>
-      <c r="L11" s="21" t="str">
+      <c r="L11" s="19" t="str">
         <f t="shared" si="0"/>
         <v>F</v>
       </c>
@@ -4435,7 +3783,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="15.75" thickBot="1">
+    <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -4459,7 +3807,7 @@
         <f t="shared" si="0"/>
         <v>F</v>
       </c>
-      <c r="L12" s="21" t="str">
+      <c r="L12" s="19" t="str">
         <f t="shared" si="0"/>
         <v>F</v>
       </c>
@@ -4483,54 +3831,54 @@
         <f t="shared" si="0"/>
         <v>F</v>
       </c>
-      <c r="R12" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>F</v>
-      </c>
-      <c r="S12" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>F</v>
-      </c>
-      <c r="T12" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>F</v>
-      </c>
-      <c r="U12" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>F</v>
-      </c>
-      <c r="V12" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>F</v>
-      </c>
-      <c r="W12" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>F</v>
-      </c>
-      <c r="X12" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>F</v>
-      </c>
-      <c r="Y12" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>F</v>
-      </c>
-      <c r="Z12" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>F</v>
-      </c>
-      <c r="AA12" s="23" t="str">
+      <c r="R12" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+      <c r="S12" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+      <c r="T12" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+      <c r="U12" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+      <c r="V12" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+      <c r="W12" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+      <c r="X12" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+      <c r="Y12" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+      <c r="Z12" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+      <c r="AA12" s="21" t="str">
         <f t="shared" si="1"/>
         <v>F</v>
       </c>
     </row>
-    <row r="13" spans="1:27">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
-      <c r="B13" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
+      <c r="B13" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
       <c r="E13" s="1"/>
       <c r="G13" s="3">
         <v>11</v>
@@ -4551,7 +3899,7 @@
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-      <c r="L13" s="21" t="str">
+      <c r="L13" s="19" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
@@ -4571,7 +3919,7 @@
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-      <c r="Q13" s="21" t="str">
+      <c r="Q13" s="19" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
@@ -4616,7 +3964,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="14" spans="1:27">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="18">
         <v>1</v>
       </c>
@@ -4655,7 +4003,7 @@
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-      <c r="L14" s="21" t="str">
+      <c r="L14" s="19" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
@@ -4675,7 +4023,7 @@
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-      <c r="Q14" s="21" t="str">
+      <c r="Q14" s="19" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
@@ -4720,7 +4068,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="18">
         <v>2</v>
       </c>
@@ -4759,7 +4107,7 @@
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-      <c r="L15" s="21" t="str">
+      <c r="L15" s="19" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
@@ -4779,7 +4127,7 @@
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-      <c r="Q15" s="21" t="str">
+      <c r="Q15" s="19" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
@@ -4824,7 +4172,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="16" spans="1:27">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="18">
         <v>3</v>
       </c>
@@ -4863,7 +4211,7 @@
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-      <c r="L16" s="21" t="str">
+      <c r="L16" s="19" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
@@ -4883,7 +4231,7 @@
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-      <c r="Q16" s="21" t="str">
+      <c r="Q16" s="19" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
@@ -4928,7 +4276,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="15.75" thickBot="1">
+    <row r="17" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18">
         <v>4</v>
       </c>
@@ -4967,7 +4315,7 @@
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-      <c r="L17" s="21" t="str">
+      <c r="L17" s="19" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
@@ -4987,7 +4335,7 @@
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-      <c r="Q17" s="21" t="str">
+      <c r="Q17" s="19" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
@@ -5011,28 +4359,28 @@
         <f t="shared" si="3"/>
         <v>F</v>
       </c>
-      <c r="W17" s="22" t="str">
-        <f t="shared" si="3"/>
-        <v>F</v>
-      </c>
-      <c r="X17" s="22" t="str">
-        <f t="shared" si="3"/>
-        <v>F</v>
-      </c>
-      <c r="Y17" s="22" t="str">
-        <f t="shared" si="3"/>
-        <v>F</v>
-      </c>
-      <c r="Z17" s="22" t="str">
-        <f t="shared" si="3"/>
-        <v>F</v>
-      </c>
-      <c r="AA17" s="23" t="str">
+      <c r="W17" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+      <c r="X17" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+      <c r="Y17" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+      <c r="Z17" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+      <c r="AA17" s="21" t="str">
         <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
-    <row r="18" spans="1:27">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -5056,7 +4404,7 @@
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-      <c r="L18" s="21" t="str">
+      <c r="L18" s="19" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
@@ -5076,7 +4424,7 @@
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-      <c r="Q18" s="21" t="str">
+      <c r="Q18" s="19" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
@@ -5096,7 +4444,7 @@
         <f t="shared" si="3"/>
         <v>F</v>
       </c>
-      <c r="V18" s="21" t="str">
+      <c r="V18" s="19" t="str">
         <f t="shared" si="3"/>
         <v>F</v>
       </c>
@@ -5121,13 +4469,13 @@
         <v>F</v>
       </c>
     </row>
-    <row r="19" spans="1:27">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
-      <c r="B19" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
+      <c r="B19" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
       <c r="E19" s="1"/>
       <c r="G19" s="3">
         <v>17</v>
@@ -5148,7 +4496,7 @@
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-      <c r="L19" s="21" t="str">
+      <c r="L19" s="19" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
@@ -5168,7 +4516,7 @@
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-      <c r="Q19" s="21" t="str">
+      <c r="Q19" s="19" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
@@ -5188,7 +4536,7 @@
         <f t="shared" si="3"/>
         <v>F</v>
       </c>
-      <c r="V19" s="21" t="str">
+      <c r="V19" s="19" t="str">
         <f t="shared" si="3"/>
         <v>F</v>
       </c>
@@ -5213,7 +4561,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="20" spans="1:27">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="18">
         <v>1</v>
       </c>
@@ -5252,7 +4600,7 @@
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-      <c r="L20" s="21" t="str">
+      <c r="L20" s="19" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
@@ -5272,7 +4620,7 @@
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-      <c r="Q20" s="21" t="str">
+      <c r="Q20" s="19" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
@@ -5292,7 +4640,7 @@
         <f t="shared" si="3"/>
         <v>F</v>
       </c>
-      <c r="V20" s="21" t="str">
+      <c r="V20" s="19" t="str">
         <f t="shared" si="3"/>
         <v>F</v>
       </c>
@@ -5317,7 +4665,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="21" spans="1:27">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="18">
         <v>2</v>
       </c>
@@ -5356,7 +4704,7 @@
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-      <c r="L21" s="21" t="str">
+      <c r="L21" s="19" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
@@ -5376,7 +4724,7 @@
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-      <c r="Q21" s="21" t="str">
+      <c r="Q21" s="19" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
@@ -5396,7 +4744,7 @@
         <f t="shared" si="3"/>
         <v>F</v>
       </c>
-      <c r="V21" s="21" t="str">
+      <c r="V21" s="19" t="str">
         <f t="shared" si="3"/>
         <v>F</v>
       </c>
@@ -5421,7 +4769,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="22" spans="1:27" ht="15.75" thickBot="1">
+    <row r="22" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18">
         <v>3</v>
       </c>
@@ -5460,7 +4808,7 @@
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-      <c r="L22" s="24" t="str">
+      <c r="L22" s="22" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
@@ -5480,7 +4828,7 @@
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-      <c r="Q22" s="24" t="str">
+      <c r="Q22" s="22" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
@@ -5500,7 +4848,7 @@
         <f t="shared" si="3"/>
         <v>F</v>
       </c>
-      <c r="V22" s="24" t="str">
+      <c r="V22" s="22" t="str">
         <f t="shared" si="3"/>
         <v>F</v>
       </c>
@@ -5525,7 +4873,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="23" spans="1:27">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="18">
         <v>4</v>
       </c>
@@ -5552,18 +4900,18 @@
     <mergeCell ref="B19:D19"/>
   </mergeCells>
   <conditionalFormatting sqref="B14:E17 B20:E23">
-    <cfRule type="cellIs" dxfId="35" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"V"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:AA22">
-    <cfRule type="cellIs" dxfId="33" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"V"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5572,676 +4920,676 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="10" width="5.7109375" customWidth="1"/>
     <col min="11" max="11" width="10.7109375" customWidth="1"/>
     <col min="12" max="21" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="30" customHeight="1" thickBot="1">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="33">
+        <v>1</v>
+      </c>
+      <c r="C1" s="33">
+        <v>2</v>
+      </c>
+      <c r="D1" s="33">
         <v>3</v>
       </c>
-      <c r="B1" s="37">
-        <v>1</v>
-      </c>
-      <c r="C1" s="37">
+      <c r="E1" s="33">
+        <v>4</v>
+      </c>
+      <c r="F1" s="33">
+        <v>5</v>
+      </c>
+      <c r="G1" s="33">
+        <v>6</v>
+      </c>
+      <c r="H1" s="33">
+        <v>7</v>
+      </c>
+      <c r="I1" s="33">
+        <v>8</v>
+      </c>
+      <c r="J1" s="33">
+        <v>9</v>
+      </c>
+      <c r="K1" s="23"/>
+      <c r="L1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" s="33">
+        <v>1</v>
+      </c>
+      <c r="N1" s="33">
         <v>2</v>
       </c>
-      <c r="D1" s="37">
+      <c r="O1" s="33">
         <v>3</v>
       </c>
-      <c r="E1" s="37">
+      <c r="P1" s="33">
         <v>4</v>
       </c>
-      <c r="F1" s="37">
+      <c r="Q1" s="33">
         <v>5</v>
       </c>
-      <c r="G1" s="37">
+      <c r="R1" s="33">
         <v>6</v>
       </c>
-      <c r="H1" s="37">
+      <c r="S1" s="33">
         <v>7</v>
       </c>
-      <c r="I1" s="37">
+      <c r="T1" s="33">
         <v>8</v>
       </c>
-      <c r="J1" s="37">
+      <c r="U1" s="33">
         <v>9</v>
       </c>
-      <c r="K1" s="27"/>
-      <c r="L1" s="37" t="s">
+    </row>
+    <row r="2" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="33">
+        <v>1</v>
+      </c>
+      <c r="B2" s="25">
+        <v>1</v>
+      </c>
+      <c r="C2" s="26">
+        <v>1</v>
+      </c>
+      <c r="D2" s="26">
+        <v>1</v>
+      </c>
+      <c r="E2" s="26">
+        <v>1</v>
+      </c>
+      <c r="F2" s="26">
+        <v>1</v>
+      </c>
+      <c r="G2" s="26">
+        <v>1</v>
+      </c>
+      <c r="H2" s="26">
+        <v>1</v>
+      </c>
+      <c r="I2" s="26">
+        <v>1</v>
+      </c>
+      <c r="J2" s="27">
+        <v>1</v>
+      </c>
+      <c r="L2" s="33">
+        <v>1</v>
+      </c>
+      <c r="M2" s="25">
+        <v>1</v>
+      </c>
+      <c r="N2" s="26">
+        <v>1</v>
+      </c>
+      <c r="O2" s="26">
+        <v>1</v>
+      </c>
+      <c r="P2" s="26">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="26">
+        <f>IF(AND(Q5=0,Q4=0,Q3=0,F3=0),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="R2" s="26">
+        <v>1</v>
+      </c>
+      <c r="S2" s="26">
+        <v>1</v>
+      </c>
+      <c r="T2" s="26">
+        <v>1</v>
+      </c>
+      <c r="U2" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33">
+        <v>2</v>
+      </c>
+      <c r="B3" s="28">
+        <v>1</v>
+      </c>
+      <c r="C3" s="24">
+        <v>0</v>
+      </c>
+      <c r="D3" s="24">
+        <v>0</v>
+      </c>
+      <c r="E3" s="24">
+        <v>0</v>
+      </c>
+      <c r="F3" s="24">
+        <v>0</v>
+      </c>
+      <c r="G3" s="24">
+        <v>0</v>
+      </c>
+      <c r="H3" s="24">
+        <v>0</v>
+      </c>
+      <c r="I3" s="24">
+        <v>0</v>
+      </c>
+      <c r="J3" s="29">
+        <v>1</v>
+      </c>
+      <c r="L3" s="33">
+        <v>2</v>
+      </c>
+      <c r="M3" s="28">
+        <v>1</v>
+      </c>
+      <c r="N3" s="24">
+        <v>1</v>
+      </c>
+      <c r="O3" s="24">
+        <v>1</v>
+      </c>
+      <c r="P3" s="24">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="24">
+        <f>IF(AND(Q5=0,Q4=0,F4=0),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="R3" s="24">
+        <v>1</v>
+      </c>
+      <c r="S3" s="24">
+        <v>1</v>
+      </c>
+      <c r="T3" s="24">
+        <v>1</v>
+      </c>
+      <c r="U3" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="33">
         <v>3</v>
       </c>
-      <c r="M1" s="37">
-        <v>1</v>
-      </c>
-      <c r="N1" s="37">
-        <v>2</v>
-      </c>
-      <c r="O1" s="37">
+      <c r="B4" s="28">
+        <v>1</v>
+      </c>
+      <c r="C4" s="24">
+        <v>0</v>
+      </c>
+      <c r="D4" s="24">
+        <v>0</v>
+      </c>
+      <c r="E4" s="24">
+        <v>0</v>
+      </c>
+      <c r="F4" s="24">
+        <v>0</v>
+      </c>
+      <c r="G4" s="24">
+        <v>0</v>
+      </c>
+      <c r="H4" s="24">
+        <v>0</v>
+      </c>
+      <c r="I4" s="24">
+        <v>0</v>
+      </c>
+      <c r="J4" s="29">
+        <v>1</v>
+      </c>
+      <c r="L4" s="33">
         <v>3</v>
       </c>
-      <c r="P1" s="37">
+      <c r="M4" s="28">
+        <v>1</v>
+      </c>
+      <c r="N4" s="24">
+        <v>1</v>
+      </c>
+      <c r="O4" s="24">
+        <f>IF(OR(AND(O5=0,E5=0),AND(P4=0,E5=0)),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="24">
+        <f>IF(OR(AND(Q5=0,P5=0,E5=0),AND(Q5=0,Q4=0,F4=0)),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="24">
+        <f>IF(AND(Q5=0,F5=0),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="R4" s="24">
+        <f>IF(OR(AND(Q5=0,Q4=0,F4=0),AND(Q5=0,R5=0,G5=0)),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="S4" s="24">
+        <f>IF(OR(AND(S5=0,G5=0),AND(R4=0,G5=0)),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="T4" s="24">
+        <v>1</v>
+      </c>
+      <c r="U4" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="33">
         <v>4</v>
       </c>
-      <c r="Q1" s="37">
+      <c r="B5" s="28">
+        <v>1</v>
+      </c>
+      <c r="C5" s="24">
+        <v>0</v>
+      </c>
+      <c r="D5" s="24">
+        <v>0</v>
+      </c>
+      <c r="E5" s="24">
+        <v>0</v>
+      </c>
+      <c r="F5" s="24">
+        <v>0</v>
+      </c>
+      <c r="G5" s="24">
+        <v>0</v>
+      </c>
+      <c r="H5" s="24">
+        <v>0</v>
+      </c>
+      <c r="I5" s="24">
+        <v>0</v>
+      </c>
+      <c r="J5" s="29">
+        <v>1</v>
+      </c>
+      <c r="L5" s="33">
+        <v>4</v>
+      </c>
+      <c r="M5" s="28">
+        <v>1</v>
+      </c>
+      <c r="N5" s="24">
+        <v>1</v>
+      </c>
+      <c r="O5" s="24">
+        <f>IF(OR(AND(P6=0,P5=0),AND(P6=0,O6=0)),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="P5" s="24">
+        <f>IF(OR(E6=0,F5=0),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="24">
+        <v>0</v>
+      </c>
+      <c r="R5" s="24">
+        <f>IF(OR(G6=0,F5=0),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="S5" s="24">
+        <f>IF(OR(AND(R6=0,R5=0),AND(R6=0,S6=0)),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="T5" s="24">
+        <v>1</v>
+      </c>
+      <c r="U5" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="33">
         <v>5</v>
       </c>
-      <c r="R1" s="37">
+      <c r="B6" s="28">
+        <v>1</v>
+      </c>
+      <c r="C6" s="24">
+        <v>0</v>
+      </c>
+      <c r="D6" s="24">
+        <v>0</v>
+      </c>
+      <c r="E6" s="24">
+        <v>0</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="24">
+        <v>0</v>
+      </c>
+      <c r="H6" s="24">
+        <v>0</v>
+      </c>
+      <c r="I6" s="24">
+        <v>0</v>
+      </c>
+      <c r="J6" s="29">
+        <v>1</v>
+      </c>
+      <c r="L6" s="33">
+        <v>5</v>
+      </c>
+      <c r="M6" s="28">
+        <f>IF(AND(O6=0,P6=0,N6=0,C6=0),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="24">
+        <f>IF(AND(P6=0,O6=0,D6=0),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="24">
+        <f>IF(AND(P6=0,E6=0),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="P6" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="R6" s="24">
+        <v>0</v>
+      </c>
+      <c r="S6" s="24">
+        <f>IF(AND(R6=0,G6=0),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="T6" s="24">
+        <f>IF(AND(S6=0,R6=0,H6=0),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="U6" s="29">
+        <f>IF(AND(T6=0,S6=0,R6=0,I6=0),0,1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="33">
         <v>6</v>
       </c>
-      <c r="S1" s="37">
+      <c r="B7" s="28">
+        <v>1</v>
+      </c>
+      <c r="C7" s="24">
+        <v>0</v>
+      </c>
+      <c r="D7" s="24">
+        <v>0</v>
+      </c>
+      <c r="E7" s="24">
+        <v>0</v>
+      </c>
+      <c r="F7" s="24">
+        <v>0</v>
+      </c>
+      <c r="G7" s="24">
+        <v>0</v>
+      </c>
+      <c r="H7" s="24">
+        <v>0</v>
+      </c>
+      <c r="I7" s="24">
+        <v>0</v>
+      </c>
+      <c r="J7" s="29">
+        <v>1</v>
+      </c>
+      <c r="L7" s="33">
+        <v>6</v>
+      </c>
+      <c r="M7" s="28">
+        <v>1</v>
+      </c>
+      <c r="N7" s="24">
+        <v>1</v>
+      </c>
+      <c r="O7" s="24">
+        <f>IF(OR(AND(P6=0,O6=0),AND(P7=0,P6=0)),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="24">
+        <f>IF(OR(E6=0,F7=0),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="24">
+        <v>0</v>
+      </c>
+      <c r="R7" s="24">
+        <f>IF(OR(F7=0,G6=0),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="S7" s="24">
+        <f>IF(OR(AND(S6=0,R7=0),AND(R7=0,R6=0)),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="T7" s="24">
+        <v>1</v>
+      </c>
+      <c r="U7" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="33">
         <v>7</v>
       </c>
-      <c r="T1" s="37">
+      <c r="B8" s="28">
+        <v>1</v>
+      </c>
+      <c r="C8" s="24">
+        <v>0</v>
+      </c>
+      <c r="D8" s="24">
+        <v>0</v>
+      </c>
+      <c r="E8" s="24">
+        <v>0</v>
+      </c>
+      <c r="F8" s="24">
+        <v>0</v>
+      </c>
+      <c r="G8" s="24">
+        <v>0</v>
+      </c>
+      <c r="H8" s="24">
+        <v>0</v>
+      </c>
+      <c r="I8" s="24">
+        <v>0</v>
+      </c>
+      <c r="J8" s="29">
+        <v>1</v>
+      </c>
+      <c r="L8" s="33">
+        <v>7</v>
+      </c>
+      <c r="M8" s="28">
+        <v>1</v>
+      </c>
+      <c r="N8" s="24">
+        <v>1</v>
+      </c>
+      <c r="O8" s="24">
+        <f>IF(OR(AND(P8=0,E7=0),AND(O7=0,E7=0)),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="P8" s="24">
+        <f>IF(OR(AND(Q7=0,P7=0,E7=0),AND(Q7=0,Q8=0,F8=0)),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="24">
+        <f>IF(AND(Q7=0,F7=0),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="R8" s="24">
+        <f>IF(OR(AND(Q7=0,Q8=0,F8=0),AND(Q7=0,R7=0,G7=0)),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="S8" s="24">
+        <f>IF(OR(AND(S7=0,G7=0),AND(R8=0,G7=0)),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="T8" s="24">
+        <v>1</v>
+      </c>
+      <c r="U8" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="33">
         <v>8</v>
       </c>
-      <c r="U1" s="37">
+      <c r="B9" s="28">
+        <v>1</v>
+      </c>
+      <c r="C9" s="24">
+        <v>0</v>
+      </c>
+      <c r="D9" s="24">
+        <v>0</v>
+      </c>
+      <c r="E9" s="24">
+        <v>0</v>
+      </c>
+      <c r="F9" s="24">
+        <v>0</v>
+      </c>
+      <c r="G9" s="24">
+        <v>0</v>
+      </c>
+      <c r="H9" s="24">
+        <v>0</v>
+      </c>
+      <c r="I9" s="24">
+        <v>0</v>
+      </c>
+      <c r="J9" s="29">
+        <v>1</v>
+      </c>
+      <c r="L9" s="33">
+        <v>8</v>
+      </c>
+      <c r="M9" s="28">
+        <v>1</v>
+      </c>
+      <c r="N9" s="24">
+        <v>1</v>
+      </c>
+      <c r="O9" s="24">
+        <v>1</v>
+      </c>
+      <c r="P9" s="24">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="24">
+        <f>IF(AND(Q7=0,Q8=0,F8=0),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="R9" s="24">
+        <v>1</v>
+      </c>
+      <c r="S9" s="24">
+        <v>1</v>
+      </c>
+      <c r="T9" s="24">
+        <v>1</v>
+      </c>
+      <c r="U9" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="33">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" ht="30" customHeight="1">
-      <c r="A2" s="37">
-        <v>1</v>
-      </c>
-      <c r="B2" s="29">
-        <v>1</v>
-      </c>
-      <c r="C2" s="30">
-        <v>1</v>
-      </c>
-      <c r="D2" s="30">
-        <v>1</v>
-      </c>
-      <c r="E2" s="30">
-        <v>1</v>
-      </c>
-      <c r="F2" s="30">
-        <v>1</v>
-      </c>
-      <c r="G2" s="30">
-        <v>1</v>
-      </c>
-      <c r="H2" s="30">
-        <v>1</v>
-      </c>
-      <c r="I2" s="30">
-        <v>1</v>
-      </c>
-      <c r="J2" s="31">
-        <v>1</v>
-      </c>
-      <c r="L2" s="37">
-        <v>1</v>
-      </c>
-      <c r="M2" s="29">
-        <v>1</v>
-      </c>
-      <c r="N2" s="30">
-        <v>1</v>
-      </c>
-      <c r="O2" s="30">
-        <v>1</v>
-      </c>
-      <c r="P2" s="30">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="30">
-        <f>IF(AND(Q5=0,Q4=0,Q3=0,F3=0),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="R2" s="30">
-        <v>1</v>
-      </c>
-      <c r="S2" s="30">
-        <v>1</v>
-      </c>
-      <c r="T2" s="30">
-        <v>1</v>
-      </c>
-      <c r="U2" s="31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="30" customHeight="1">
-      <c r="A3" s="37">
-        <v>2</v>
-      </c>
-      <c r="B3" s="32">
-        <v>1</v>
-      </c>
-      <c r="C3" s="28">
-        <v>0</v>
-      </c>
-      <c r="D3" s="28">
-        <v>0</v>
-      </c>
-      <c r="E3" s="28">
-        <v>0</v>
-      </c>
-      <c r="F3" s="28">
-        <v>0</v>
-      </c>
-      <c r="G3" s="28">
-        <v>0</v>
-      </c>
-      <c r="H3" s="28">
-        <v>0</v>
-      </c>
-      <c r="I3" s="28">
-        <v>0</v>
-      </c>
-      <c r="J3" s="33">
-        <v>1</v>
-      </c>
-      <c r="L3" s="37">
-        <v>2</v>
-      </c>
-      <c r="M3" s="32">
-        <v>1</v>
-      </c>
-      <c r="N3" s="28">
-        <v>1</v>
-      </c>
-      <c r="O3" s="28">
-        <v>1</v>
-      </c>
-      <c r="P3" s="28">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="28">
-        <f>IF(AND(Q5=0,Q4=0,F4=0),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="R3" s="28">
-        <v>1</v>
-      </c>
-      <c r="S3" s="28">
-        <v>1</v>
-      </c>
-      <c r="T3" s="28">
-        <v>1</v>
-      </c>
-      <c r="U3" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="30" customHeight="1">
-      <c r="A4" s="37">
-        <v>3</v>
-      </c>
-      <c r="B4" s="32">
-        <v>1</v>
-      </c>
-      <c r="C4" s="28">
-        <v>0</v>
-      </c>
-      <c r="D4" s="28">
-        <v>0</v>
-      </c>
-      <c r="E4" s="28">
-        <v>0</v>
-      </c>
-      <c r="F4" s="28">
-        <v>0</v>
-      </c>
-      <c r="G4" s="28">
-        <v>0</v>
-      </c>
-      <c r="H4" s="28">
-        <v>0</v>
-      </c>
-      <c r="I4" s="28">
-        <v>0</v>
-      </c>
-      <c r="J4" s="33">
-        <v>1</v>
-      </c>
-      <c r="L4" s="37">
-        <v>3</v>
-      </c>
-      <c r="M4" s="32">
-        <v>1</v>
-      </c>
-      <c r="N4" s="28">
-        <v>1</v>
-      </c>
-      <c r="O4" s="28">
-        <f>IF(OR(AND(O5=0,E5=0),AND(P4=0,E5=0)),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="P4" s="28">
-        <f>IF(OR(AND(Q5=0,P5=0,E5=0),AND(Q5=0,Q4=0,F4=0)),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="Q4" s="28">
-        <f>IF(AND(Q5=0,F5=0),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="R4" s="28">
-        <f>IF(OR(AND(Q5=0,Q4=0,F4=0),AND(Q5=0,R5=0,G5=0)),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="S4" s="28">
-        <f>IF(OR(AND(S5=0,G5=0),AND(R4=0,G5=0)),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="T4" s="28">
-        <v>1</v>
-      </c>
-      <c r="U4" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="30" customHeight="1">
-      <c r="A5" s="37">
-        <v>4</v>
-      </c>
-      <c r="B5" s="32">
-        <v>1</v>
-      </c>
-      <c r="C5" s="28">
-        <v>0</v>
-      </c>
-      <c r="D5" s="28">
-        <v>0</v>
-      </c>
-      <c r="E5" s="28">
-        <v>0</v>
-      </c>
-      <c r="F5" s="28">
-        <v>0</v>
-      </c>
-      <c r="G5" s="28">
-        <v>0</v>
-      </c>
-      <c r="H5" s="28">
-        <v>0</v>
-      </c>
-      <c r="I5" s="28">
-        <v>0</v>
-      </c>
-      <c r="J5" s="33">
-        <v>1</v>
-      </c>
-      <c r="L5" s="37">
-        <v>4</v>
-      </c>
-      <c r="M5" s="32">
-        <v>1</v>
-      </c>
-      <c r="N5" s="28">
-        <v>1</v>
-      </c>
-      <c r="O5" s="28">
-        <f>IF(OR(AND(P6=0,P5=0),AND(P6=0,O6=0)),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="P5" s="28">
-        <f>IF(OR(E6=0,F5=0),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="28">
-        <v>0</v>
-      </c>
-      <c r="R5" s="28">
-        <f>IF(OR(G6=0,F5=0),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="S5" s="28">
-        <f>IF(OR(AND(R6=0,R5=0),AND(R6=0,S6=0)),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="T5" s="28">
-        <v>1</v>
-      </c>
-      <c r="U5" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="30" customHeight="1">
-      <c r="A6" s="37">
-        <v>5</v>
-      </c>
-      <c r="B6" s="32">
-        <v>1</v>
-      </c>
-      <c r="C6" s="28">
-        <v>0</v>
-      </c>
-      <c r="D6" s="28">
-        <v>0</v>
-      </c>
-      <c r="E6" s="28">
-        <v>0</v>
-      </c>
-      <c r="F6" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="28">
-        <v>0</v>
-      </c>
-      <c r="H6" s="28">
-        <v>0</v>
-      </c>
-      <c r="I6" s="28">
-        <v>0</v>
-      </c>
-      <c r="J6" s="33">
-        <v>1</v>
-      </c>
-      <c r="L6" s="37">
-        <v>5</v>
-      </c>
-      <c r="M6" s="32">
-        <f>IF(AND(O6=0,P6=0,N6=0,C6=0),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="N6" s="28">
-        <f>IF(AND(P6=0,O6=0,D6=0),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="O6" s="28">
-        <f>IF(AND(P6=0,E6=0),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="P6" s="28">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="R6" s="28">
-        <v>0</v>
-      </c>
-      <c r="S6" s="28">
-        <f>IF(AND(R6=0,G6=0),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="T6" s="28">
-        <f>IF(AND(S6=0,R6=0,H6=0),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="U6" s="33">
-        <f>IF(AND(T6=0,S6=0,R6=0,I6=0),0,1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="30" customHeight="1">
-      <c r="A7" s="37">
-        <v>6</v>
-      </c>
-      <c r="B7" s="32">
-        <v>1</v>
-      </c>
-      <c r="C7" s="28">
-        <v>0</v>
-      </c>
-      <c r="D7" s="28">
-        <v>0</v>
-      </c>
-      <c r="E7" s="28">
-        <v>0</v>
-      </c>
-      <c r="F7" s="28">
-        <v>0</v>
-      </c>
-      <c r="G7" s="28">
-        <v>0</v>
-      </c>
-      <c r="H7" s="28">
-        <v>0</v>
-      </c>
-      <c r="I7" s="28">
-        <v>0</v>
-      </c>
-      <c r="J7" s="33">
-        <v>1</v>
-      </c>
-      <c r="L7" s="37">
-        <v>6</v>
-      </c>
-      <c r="M7" s="32">
-        <v>1</v>
-      </c>
-      <c r="N7" s="28">
-        <v>1</v>
-      </c>
-      <c r="O7" s="28">
-        <f>IF(OR(AND(P6=0,O6=0),AND(P7=0,P6=0)),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="P7" s="28">
-        <f>IF(OR(E6=0,F7=0),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="Q7" s="28">
-        <v>0</v>
-      </c>
-      <c r="R7" s="28">
-        <f>IF(OR(F7=0,G6=0),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="S7" s="28">
-        <f>IF(OR(AND(S6=0,R7=0),AND(R7=0,R6=0)),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="T7" s="28">
-        <v>1</v>
-      </c>
-      <c r="U7" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" ht="30" customHeight="1">
-      <c r="A8" s="37">
-        <v>7</v>
-      </c>
-      <c r="B8" s="32">
-        <v>1</v>
-      </c>
-      <c r="C8" s="28">
-        <v>0</v>
-      </c>
-      <c r="D8" s="28">
-        <v>0</v>
-      </c>
-      <c r="E8" s="28">
-        <v>0</v>
-      </c>
-      <c r="F8" s="28">
-        <v>0</v>
-      </c>
-      <c r="G8" s="28">
-        <v>0</v>
-      </c>
-      <c r="H8" s="28">
-        <v>0</v>
-      </c>
-      <c r="I8" s="28">
-        <v>0</v>
-      </c>
-      <c r="J8" s="33">
-        <v>1</v>
-      </c>
-      <c r="L8" s="37">
-        <v>7</v>
-      </c>
-      <c r="M8" s="32">
-        <v>1</v>
-      </c>
-      <c r="N8" s="28">
-        <v>1</v>
-      </c>
-      <c r="O8" s="28">
-        <f>IF(OR(AND(P8=0,E7=0),AND(O7=0,E7=0)),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="P8" s="28">
-        <f>IF(OR(AND(Q7=0,P7=0,E7=0),AND(Q7=0,Q8=0,F8=0)),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="Q8" s="28">
-        <f>IF(AND(Q7=0,F7=0),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="R8" s="28">
-        <f>IF(OR(AND(Q7=0,Q8=0,F8=0),AND(Q7=0,R7=0,G7=0)),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="S8" s="28">
-        <f>IF(OR(AND(S7=0,G7=0),AND(R8=0,G7=0)),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="T8" s="28">
-        <v>1</v>
-      </c>
-      <c r="U8" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" ht="30" customHeight="1">
-      <c r="A9" s="37">
-        <v>8</v>
-      </c>
-      <c r="B9" s="32">
-        <v>1</v>
-      </c>
-      <c r="C9" s="28">
-        <v>0</v>
-      </c>
-      <c r="D9" s="28">
-        <v>0</v>
-      </c>
-      <c r="E9" s="28">
-        <v>0</v>
-      </c>
-      <c r="F9" s="28">
-        <v>0</v>
-      </c>
-      <c r="G9" s="28">
-        <v>0</v>
-      </c>
-      <c r="H9" s="28">
-        <v>0</v>
-      </c>
-      <c r="I9" s="28">
-        <v>0</v>
-      </c>
-      <c r="J9" s="33">
-        <v>1</v>
-      </c>
-      <c r="L9" s="37">
-        <v>8</v>
-      </c>
-      <c r="M9" s="32">
-        <v>1</v>
-      </c>
-      <c r="N9" s="28">
-        <v>1</v>
-      </c>
-      <c r="O9" s="28">
-        <v>1</v>
-      </c>
-      <c r="P9" s="28">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="28">
-        <f>IF(AND(Q7=0,Q8=0,F8=0),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="R9" s="28">
-        <v>1</v>
-      </c>
-      <c r="S9" s="28">
-        <v>1</v>
-      </c>
-      <c r="T9" s="28">
-        <v>1</v>
-      </c>
-      <c r="U9" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" ht="30" customHeight="1" thickBot="1">
-      <c r="A10" s="37">
+      <c r="B10" s="30">
+        <v>1</v>
+      </c>
+      <c r="C10" s="31">
+        <v>1</v>
+      </c>
+      <c r="D10" s="31">
+        <v>1</v>
+      </c>
+      <c r="E10" s="31">
+        <v>1</v>
+      </c>
+      <c r="F10" s="31">
+        <v>1</v>
+      </c>
+      <c r="G10" s="31">
+        <v>1</v>
+      </c>
+      <c r="H10" s="31">
+        <v>1</v>
+      </c>
+      <c r="I10" s="31">
+        <v>1</v>
+      </c>
+      <c r="J10" s="32">
+        <v>1</v>
+      </c>
+      <c r="L10" s="33">
         <v>9</v>
       </c>
-      <c r="B10" s="34">
-        <v>1</v>
-      </c>
-      <c r="C10" s="35">
-        <v>1</v>
-      </c>
-      <c r="D10" s="35">
-        <v>1</v>
-      </c>
-      <c r="E10" s="35">
-        <v>1</v>
-      </c>
-      <c r="F10" s="35">
-        <v>1</v>
-      </c>
-      <c r="G10" s="35">
-        <v>1</v>
-      </c>
-      <c r="H10" s="35">
-        <v>1</v>
-      </c>
-      <c r="I10" s="35">
-        <v>1</v>
-      </c>
-      <c r="J10" s="36">
-        <v>1</v>
-      </c>
-      <c r="L10" s="37">
-        <v>9</v>
-      </c>
-      <c r="M10" s="34">
-        <v>1</v>
-      </c>
-      <c r="N10" s="35">
-        <v>1</v>
-      </c>
-      <c r="O10" s="35">
-        <v>1</v>
-      </c>
-      <c r="P10" s="35">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="35">
+      <c r="M10" s="30">
+        <v>1</v>
+      </c>
+      <c r="N10" s="31">
+        <v>1</v>
+      </c>
+      <c r="O10" s="31">
+        <v>1</v>
+      </c>
+      <c r="P10" s="31">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="31">
         <f>IF(AND(Q9=0,Q8=0,Q7=0,F9=0),0,1)</f>
         <v>0</v>
       </c>
-      <c r="R10" s="35">
-        <v>1</v>
-      </c>
-      <c r="S10" s="35">
-        <v>1</v>
-      </c>
-      <c r="T10" s="35">
-        <v>1</v>
-      </c>
-      <c r="U10" s="36">
+      <c r="R10" s="31">
+        <v>1</v>
+      </c>
+      <c r="S10" s="31">
+        <v>1</v>
+      </c>
+      <c r="T10" s="31">
+        <v>1</v>
+      </c>
+      <c r="U10" s="32">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="M2:U10 B2:J10">
-    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6250,13 +5598,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>